<commit_message>
modified the requirements file using venv
</commit_message>
<xml_diff>
--- a/student_data.xlsx
+++ b/student_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,286 +446,66 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1MS21cs098</t>
+          <t>1MS21cs100</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>PRATEEK M VERNEKAR</t>
+          <t>PRATISH KUMAR</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>9.33</t>
+          <t>8.23</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>9.52</t>
+          <t>8.65</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1MS21cs099</t>
+          <t>1MS21cs101</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PRATHAMESH MAHANTESH DEVARAMANI</t>
+          <t>PREETHAM M P</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>8.85</t>
+          <t>8.57</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>9.11</t>
+          <t>8.55</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1MS21cs100</t>
+          <t>1MS21cs102</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>PRATISH KUMAR</t>
+          <t>PRUTHVIRAJ M SAVANUR</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>8.23</t>
+          <t>8.71</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>8.65</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1MS21cs101</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>PREETHAM M P</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>8.57</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>8.55</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1MS21cs102</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>PRUTHVIRAJ M SAVANUR</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>8.71</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
           <t>8.80</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1MS21cs103</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>PRUTVI PRAKASH SHETTY</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>8.80</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>9.03</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1MS21cs104</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RACHNA RAMESH </t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>6.00</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>6.55</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1MS21cs105</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>RAHUL KUMAR</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>9.14</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>9.24</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>1MS21cs106</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>RAHUL RACHIPA</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1.09</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>5.94</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>1MS21cs107</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>RAKSHITHA P</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2.09</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>6.15</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>1MS21cs108</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>RIDDHIKA SAI MANOHAR</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>5.04</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>5.68</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>1MS21cs109</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>S MEENA KUMARI</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>9.61</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>9.81</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1MS21cs110</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>SAANVI NAIR</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>10.00</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>10.00</t>
         </is>
       </c>
     </row>

</xml_diff>